<commit_message>
update readme a adresy k hospodám
</commit_message>
<xml_diff>
--- a/hospody.xlsx
+++ b/hospody.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majdikleckerova/Desktop/pubmeet/pubMeet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majdikleckerova/Desktop/pubmeet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643B10EF-6FEE-1341-A77B-16C222054430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44375208-9C6D-A040-80C0-4D89FDD733D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{F4F737FC-7C70-424A-907D-C3007C0D137B}"/>
+    <workbookView xWindow="13500" yWindow="500" windowWidth="20340" windowHeight="18900" xr2:uid="{F4F737FC-7C70-424A-907D-C3007C0D137B}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Název</t>
   </si>
@@ -225,13 +225,22 @@
   </si>
   <si>
     <t>50.66150534012183</t>
+  </si>
+  <si>
+    <t>Vaníčkova Panská, 400 01 Ústí nad Labem-město</t>
+  </si>
+  <si>
+    <t>Hrnčířská 10, 400 01 Ústí nad Labem-město</t>
+  </si>
+  <si>
+    <t>Pivovarská 3380/5, 400 01 Ústí nad Labem-centrum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,6 +267,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -286,13 +301,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -630,7 +647,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,104 +677,104 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -768,10 +785,10 @@
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -779,85 +796,98 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="E14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hospody + vibe bar
</commit_message>
<xml_diff>
--- a/hospody.xlsx
+++ b/hospody.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majdikleckerova/Desktop/pubmeet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44375208-9C6D-A040-80C0-4D89FDD733D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14541E3F-E045-694E-8A40-CB7950691BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="500" windowWidth="20340" windowHeight="18900" xr2:uid="{F4F737FC-7C70-424A-907D-C3007C0D137B}"/>
+    <workbookView xWindow="12640" yWindow="620" windowWidth="20340" windowHeight="18900" xr2:uid="{F4F737FC-7C70-424A-907D-C3007C0D137B}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Název</t>
   </si>
@@ -234,6 +234,27 @@
   </si>
   <si>
     <t>Pivovarská 3380/5, 400 01 Ústí nad Labem-centrum</t>
+  </si>
+  <si>
+    <t>VIBE Lounge &amp; coctail bar</t>
+  </si>
+  <si>
+    <t>Ulice Masarykova 3125/18, 400 01 Ústí nad Labem-centrum</t>
+  </si>
+  <si>
+    <t>14.034403534402813</t>
+  </si>
+  <si>
+    <t>50.66295701796333</t>
+  </si>
+  <si>
+    <t>vibe_usti</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Telefon</t>
   </si>
 </sst>
 </file>
@@ -301,14 +322,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -644,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B2D7AA-8698-2E46-9BD8-0311C8441FEC}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,7 +679,7 @@
     <col min="5" max="5" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -675,219 +695,238 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>